<commit_message>
remove calls from diagram
</commit_message>
<xml_diff>
--- a/examples/sut_final/TestVec_30lines.xlsx
+++ b/examples/sut_final/TestVec_30lines.xlsx
@@ -402,11 +402,11 @@
       </c>
       <c r="B3" s="8">
         <f t="shared" ref="B3:D3" si="1">RANDBETWEEN(-5,5)</f>
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="C3" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D3" s="8">
         <f t="shared" si="1"/>
@@ -414,7 +414,7 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="8">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G3" s="8">
         <v>0.0</v>
@@ -430,19 +430,19 @@
       </c>
       <c r="B4" s="8">
         <f t="shared" ref="B4:D4" si="2">RANDBETWEEN(-5,5)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="8">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G4" s="8">
         <v>0.0</v>
@@ -458,19 +458,19 @@
       </c>
       <c r="B5" s="8">
         <f t="shared" ref="B5:D5" si="3">RANDBETWEEN(-5,5)</f>
-        <v>-5</v>
+        <v>2</v>
       </c>
       <c r="C5" s="8">
         <f t="shared" si="3"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
       <c r="D5" s="8">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="8">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="G5" s="8">
         <v>0.0</v>
@@ -486,19 +486,19 @@
       </c>
       <c r="B6" s="8">
         <f t="shared" ref="B6:D6" si="4">RANDBETWEEN(-5,5)</f>
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="C6" s="8">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="8">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="G6" s="8">
         <v>3.0</v>
@@ -514,19 +514,19 @@
       </c>
       <c r="B7" s="8">
         <f t="shared" ref="B7:D7" si="5">RANDBETWEEN(-5,5)</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="C7" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="D7" s="8">
         <f t="shared" si="5"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="8">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="G7" s="8">
         <v>3.0</v>
@@ -542,19 +542,19 @@
       </c>
       <c r="B8" s="8">
         <f t="shared" ref="B8:D8" si="6">RANDBETWEEN(-5,5)</f>
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="C8" s="8">
         <f t="shared" si="6"/>
-        <v>-5</v>
+        <v>1</v>
       </c>
       <c r="D8" s="8">
         <f t="shared" si="6"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="8">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c r="G8" s="8">
         <v>1.0</v>
@@ -570,19 +570,19 @@
       </c>
       <c r="B9" s="8">
         <f t="shared" ref="B9:D9" si="7">RANDBETWEEN(-5,5)</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="C9" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9" s="8">
         <f t="shared" si="7"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="8">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c r="G9" s="8">
         <v>1.0</v>
@@ -598,19 +598,19 @@
       </c>
       <c r="B10" s="8">
         <f t="shared" ref="B10:D10" si="8">RANDBETWEEN(-5,5)</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="C10" s="8">
         <f t="shared" si="8"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="D10" s="8">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="8">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G10" s="8">
         <v>1.0</v>
@@ -626,18 +626,18 @@
       </c>
       <c r="B11" s="8">
         <f t="shared" ref="B11:D11" si="9">RANDBETWEEN(-5,5)</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C11" s="8">
         <f t="shared" si="9"/>
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="D11" s="8">
         <f t="shared" si="9"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="F11" s="8">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="G11" s="8">
         <v>1.0</v>
@@ -652,18 +652,18 @@
       </c>
       <c r="B12" s="8">
         <f t="shared" ref="B12:D12" si="10">RANDBETWEEN(-5,5)</f>
-        <v>5</v>
+        <v>-5</v>
       </c>
       <c r="C12" s="8">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D12" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F12" s="8">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G12" s="8">
         <v>1.0</v>
@@ -678,18 +678,18 @@
       </c>
       <c r="B13" s="8">
         <f t="shared" ref="B13:D13" si="11">RANDBETWEEN(-5,5)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C13" s="8">
         <f t="shared" si="11"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="8">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>-5</v>
       </c>
       <c r="F13" s="8">
-        <v>0.0</v>
+        <v>11.0</v>
       </c>
       <c r="G13" s="8">
         <v>1.0</v>
@@ -704,18 +704,18 @@
       </c>
       <c r="B14" s="8">
         <f t="shared" ref="B14:D14" si="12">RANDBETWEEN(-5,5)</f>
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="C14" s="8">
         <f t="shared" si="12"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="D14" s="8">
         <f t="shared" si="12"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="8">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="G14" s="8">
         <v>1.0</v>
@@ -735,10 +735,10 @@
       </c>
       <c r="D15" s="8">
         <f t="shared" si="13"/>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="F15" s="8">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
       <c r="G15" s="8">
         <v>1.0</v>
@@ -753,18 +753,18 @@
       </c>
       <c r="B16" s="8">
         <f t="shared" ref="B16:D16" si="14">RANDBETWEEN(-5,5)</f>
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="C16" s="8">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D16" s="8">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="8">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="G16" s="8">
         <v>1.0</v>
@@ -779,18 +779,18 @@
       </c>
       <c r="B17" s="8">
         <f t="shared" ref="B17:D17" si="15">RANDBETWEEN(-5,5)</f>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="C17" s="8">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>-5</v>
       </c>
       <c r="F17" s="8">
-        <v>0.0</v>
+        <v>15.0</v>
       </c>
       <c r="G17" s="8">
         <v>1.0</v>
@@ -805,18 +805,18 @@
       </c>
       <c r="B18" s="8">
         <f t="shared" ref="B18:D18" si="16">RANDBETWEEN(-5,5)</f>
-        <v>2</v>
+        <v>-4</v>
       </c>
       <c r="C18" s="8">
         <f t="shared" si="16"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="8">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F18" s="8">
-        <v>0.0</v>
+        <v>16.0</v>
       </c>
       <c r="G18" s="8">
         <v>1.0</v>
@@ -831,18 +831,18 @@
       </c>
       <c r="B19" s="8">
         <f t="shared" ref="B19:D19" si="17">RANDBETWEEN(-5,5)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="8">
         <f t="shared" si="17"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D19" s="8">
         <f t="shared" si="17"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="8">
-        <v>0.0</v>
+        <v>17.0</v>
       </c>
       <c r="G19" s="8">
         <v>1.0</v>
@@ -857,18 +857,18 @@
       </c>
       <c r="B20" s="8">
         <f t="shared" ref="B20:D20" si="18">RANDBETWEEN(-5,5)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C20" s="8">
         <f t="shared" si="18"/>
-        <v>2</v>
+        <v>-4</v>
       </c>
       <c r="D20" s="8">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F20" s="8">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c r="G20" s="8">
         <v>1.0</v>
@@ -883,7 +883,7 @@
       </c>
       <c r="B21" s="8">
         <f t="shared" ref="B21:D21" si="19">RANDBETWEEN(-5,5)</f>
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="C21" s="8">
         <f t="shared" si="19"/>
@@ -891,10 +891,10 @@
       </c>
       <c r="D21" s="8">
         <f t="shared" si="19"/>
-        <v>-4</v>
+        <v>4</v>
       </c>
       <c r="F21" s="8">
-        <v>0.0</v>
+        <v>19.0</v>
       </c>
       <c r="G21" s="8">
         <v>1.0</v>
@@ -909,18 +909,18 @@
       </c>
       <c r="B22" s="8">
         <f t="shared" ref="B22:D22" si="20">RANDBETWEEN(-5,5)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C22" s="8">
         <f t="shared" si="20"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="D22" s="8">
         <f t="shared" si="20"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F22" s="8">
-        <v>0.0</v>
+        <v>20.0</v>
       </c>
       <c r="G22" s="8">
         <v>1.0</v>
@@ -935,18 +935,18 @@
       </c>
       <c r="B23" s="8">
         <f t="shared" ref="B23:D23" si="21">RANDBETWEEN(-5,5)</f>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="C23" s="8">
         <f t="shared" si="21"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="D23" s="8">
         <f t="shared" si="21"/>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="F23" s="8">
-        <v>0.0</v>
+        <v>21.0</v>
       </c>
       <c r="G23" s="8">
         <v>1.0</v>
@@ -961,18 +961,18 @@
       </c>
       <c r="B24" s="8">
         <f t="shared" ref="B24:D24" si="22">RANDBETWEEN(-5,5)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C24" s="8">
         <f t="shared" si="22"/>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="D24" s="8">
         <f t="shared" si="22"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F24" s="8">
-        <v>0.0</v>
+        <v>22.0</v>
       </c>
       <c r="G24" s="8">
         <v>1.0</v>
@@ -991,14 +991,14 @@
       </c>
       <c r="C25" s="8">
         <f t="shared" si="23"/>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="D25" s="8">
         <f t="shared" si="23"/>
-        <v>3</v>
+        <v>-3</v>
       </c>
       <c r="F25" s="8">
-        <v>0.0</v>
+        <v>23.0</v>
       </c>
       <c r="G25" s="8">
         <v>1.0</v>
@@ -1013,18 +1013,18 @@
       </c>
       <c r="B26" s="8">
         <f t="shared" ref="B26:D26" si="24">RANDBETWEEN(-5,5)</f>
-        <v>-4</v>
+        <v>5</v>
       </c>
       <c r="C26" s="8">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="D26" s="8">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F26" s="8">
-        <v>0.0</v>
+        <v>24.0</v>
       </c>
       <c r="G26" s="8">
         <v>1.0</v>
@@ -1039,18 +1039,18 @@
       </c>
       <c r="B27" s="8">
         <f t="shared" ref="B27:D27" si="25">RANDBETWEEN(-5,5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C27" s="8">
         <f t="shared" si="25"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="D27" s="8">
         <f t="shared" si="25"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F27" s="8">
-        <v>0.0</v>
+        <v>25.0</v>
       </c>
       <c r="G27" s="8">
         <v>1.0</v>
@@ -1065,18 +1065,18 @@
       </c>
       <c r="B28" s="8">
         <f t="shared" ref="B28:D28" si="26">RANDBETWEEN(-5,5)</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="C28" s="8">
         <f t="shared" si="26"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="D28" s="8">
         <f t="shared" si="26"/>
         <v>-2</v>
       </c>
       <c r="F28" s="8">
-        <v>0.0</v>
+        <v>26.0</v>
       </c>
       <c r="G28" s="8">
         <v>1.0</v>
@@ -1091,18 +1091,18 @@
       </c>
       <c r="B29" s="8">
         <f t="shared" ref="B29:D29" si="27">RANDBETWEEN(-5,5)</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="C29" s="8">
         <f t="shared" si="27"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D29" s="8">
         <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="F29" s="8">
-        <v>0.0</v>
+        <v>27.0</v>
       </c>
       <c r="G29" s="8">
         <v>1.0</v>
@@ -1117,18 +1117,18 @@
       </c>
       <c r="B30" s="8">
         <f t="shared" ref="B30:D30" si="28">RANDBETWEEN(-5,5)</f>
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="C30" s="8">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="D30" s="8">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="8">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="G30" s="8">
         <v>1.0</v>
@@ -1143,18 +1143,18 @@
       </c>
       <c r="B31" s="8">
         <f t="shared" ref="B31:D31" si="29">RANDBETWEEN(-5,5)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C31" s="8">
         <f t="shared" si="29"/>
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="D31" s="8">
         <f t="shared" si="29"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F31" s="8">
-        <v>0.0</v>
+        <v>29.0</v>
       </c>
       <c r="G31" s="8">
         <v>1.0</v>
@@ -1169,18 +1169,18 @@
       </c>
       <c r="B32" s="8">
         <f t="shared" ref="B32:D32" si="30">RANDBETWEEN(-5,5)</f>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="C32" s="8">
         <f t="shared" si="30"/>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="D32" s="8">
         <f t="shared" si="30"/>
-        <v>-4</v>
+        <v>5</v>
       </c>
       <c r="F32" s="8">
-        <v>0.0</v>
+        <v>30.0</v>
       </c>
       <c r="G32" s="8">
         <v>1.0</v>

</xml_diff>